<commit_message>
Partial update of writeup
</commit_message>
<xml_diff>
--- a/00-Documentation/01-WriteUp/A1-MCD/Figures/Source.xlsx
+++ b/00-Documentation/01-WriteUp/A1-MCD/Figures/Source.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/00-Documentation/01-WriteUp/A1-MCD/Figures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longkr/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/00-Documentation/01-WriteUp/A1-MCD/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F782D55-5D21-2C4C-B137-A7A50E555E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BF1706-8DCE-6A4C-90C3-616FAB709AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{7D856A4E-CAE8-ED4F-ACA2-59DB90AB5832}"/>
+    <workbookView xWindow="8640" yWindow="8620" windowWidth="27640" windowHeight="16940" xr2:uid="{7D856A4E-CAE8-ED4F-ACA2-59DB90AB5832}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$26</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="58">
   <si>
     <t>Stage</t>
   </si>
@@ -74,9 +74,6 @@
     <t>SourceMode</t>
   </si>
   <si>
-    <t>Mode</t>
-  </si>
-  <si>
     <t>SigmaX</t>
   </si>
   <si>
@@ -107,12 +104,6 @@
     <t>Maximum of energy distribution</t>
   </si>
   <si>
-    <t>nPnts</t>
-  </si>
-  <si>
-    <t>Number of points to sample for integration of PDF</t>
-  </si>
-  <si>
     <t>MinCTheta</t>
   </si>
   <si>
@@ -128,15 +119,6 @@
     <t>Laser power</t>
   </si>
   <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>Laser energy</t>
-  </si>
-  <si>
     <t>Wavelength</t>
   </si>
   <si>
@@ -161,15 +143,6 @@
     <t>Target thickness</t>
   </si>
   <si>
-    <t>Intensity</t>
-  </si>
-  <si>
-    <t>W/cm2</t>
-  </si>
-  <si>
-    <t>Laser intensity</t>
-  </si>
-  <si>
     <t>DivAngle</t>
   </si>
   <si>
@@ -204,6 +177,42 @@
   </si>
   <si>
     <t>Read particles from file</t>
+  </si>
+  <si>
+    <t>r0</t>
+  </si>
+  <si>
+    <t>Radius of laser spot</t>
+  </si>
+  <si>
+    <t>Te</t>
+  </si>
+  <si>
+    <t>Hot electron temperature</t>
+  </si>
+  <si>
+    <t>Kmin</t>
+  </si>
+  <si>
+    <t>Kmax</t>
+  </si>
+  <si>
+    <t>SigmaThetaS0</t>
+  </si>
+  <si>
+    <t>Intercept of dependence of RMS theta_S on KE</t>
+  </si>
+  <si>
+    <t>SlopeThetaS</t>
+  </si>
+  <si>
+    <t>Scaled slope of dependence of RMS theta_S on KE</t>
+  </si>
+  <si>
+    <t>rpmax</t>
+  </si>
+  <si>
+    <t>Max r prime</t>
   </si>
 </sst>
 </file>
@@ -362,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -376,6 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,10 +729,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,7 +742,7 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
   </cols>
@@ -777,14 +787,16 @@
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="H2" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -801,16 +813,16 @@
         <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F3" s="11">
-        <v>3.9999999999999998E-6</v>
+        <v>250000000000000</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -827,16 +839,16 @@
         <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="F4" s="11">
-        <v>3.9999999999999998E-6</v>
+        <v>1.5E-6</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -853,16 +865,16 @@
         <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F5" s="4">
-        <v>1</v>
+        <v>2.8000000000000001E-14</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -879,16 +891,16 @@
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="F6" s="4">
-        <v>25</v>
+        <v>2.5</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -905,14 +917,16 @@
         <v>9</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="F7" s="4">
-        <v>1000</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H7" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -929,14 +943,16 @@
         <v>9</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="F8" s="4">
-        <v>0.998</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H8" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -953,16 +969,16 @@
         <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="4">
-        <v>2500000000000000</v>
+        <v>32</v>
+      </c>
+      <c r="F9" s="11">
+        <v>3.9999999999999998E-7</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -979,16 +995,16 @@
         <v>9</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F10" s="4">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1005,16 +1021,16 @@
         <v>9</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="F11" s="4">
-        <v>0.8</v>
+        <v>20</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1031,16 +1047,16 @@
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="5">
+        <v>15</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="5">
-        <v>2.8000000000000001E-14</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="H12" s="4" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1057,92 +1073,90 @@
         <v>9</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="5">
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="G13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="13">
+        <v>-9999</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>1</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="12">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="5">
-        <v>4E+20</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>1</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="6">
-        <v>25</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
-        <v>1</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="8">
-        <v>1</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
-        <v>46</v>
+      <c r="A16" s="7">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="12">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1159,16 +1173,16 @@
         <v>9</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="12">
-        <v>3.9999999999999998E-6</v>
+        <v>38</v>
+      </c>
+      <c r="F17" s="7">
+        <v>15</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1185,116 +1199,116 @@
         <v>9</v>
       </c>
       <c r="E18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>1</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0.998</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="3">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="11">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="11">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="F18" s="12">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
-        <v>1</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="7">
-        <v>15</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>1</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
-        <v>1</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="9">
-        <v>0.998</v>
-      </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="3">
-        <v>2</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1308,19 +1322,19 @@
         <v>8</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="11">
-        <v>3.9999999999999998E-6</v>
+        <v>16</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1334,123 +1348,71 @@
         <v>8</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="11">
-        <v>3.9999999999999998E-6</v>
+        <v>19</v>
+      </c>
+      <c r="F24" s="4">
+        <v>25</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>1</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="4">
-        <v>1</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>19</v>
+      <c r="A25" s="6">
+        <v>1</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.998</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
-        <v>1</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="4">
-        <v>25</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
-        <v>1</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="6">
-        <v>0.998</v>
-      </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="10">
-        <v>1</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="10" t="s">
+      <c r="A26" s="10">
+        <v>1</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F26" s="10">
         <v>3</v>
       </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10" t="s">
-        <v>54</v>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="76" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="75" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>